<commit_message>
Update monthly sig rules under Biden
</commit_message>
<xml_diff>
--- a/data/monthly_es_rules/monthly_significant_rules_biden.xlsx
+++ b/data/monthly_es_rules/monthly_significant_rules_biden.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezd\Documents\GitHub\Reg-Stats\data\monthly_es_rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B721C5-EB0D-4A9D-BAD2-55896E902112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E843C9-53CB-4E08-8252-D427596DB966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{90C9C651-3028-4297-853F-AC0BAA5E3080}"/>
   </bookViews>
@@ -2155,7 +2155,8 @@
     <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </chartsheet>
 </file>
 
@@ -2269,6 +2270,7 @@
         <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
         <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" kern="1200">
               <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
@@ -2283,11 +2285,13 @@
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
           <a:endParaRPr lang="en-US" sz="1100" kern="1200" baseline="0">
             <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
           </a:endParaRPr>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100" kern="1200" baseline="0">
               <a:latin typeface="AvenirNext LT Pro Regular" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
@@ -2623,8 +2627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8482168B-23EE-4241-9CA4-1AEEB8D0C390}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>